<commit_message>
CIERRE 13 JUL 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #06  JUNIO  2023/BALANCE  HERRADURA  JUNIO    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #06  JUNIO  2023/BALANCE  HERRADURA  JUNIO    2023.xlsx
@@ -385,7 +385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="370">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1502,6 +1502,12 @@
   </si>
   <si>
     <t>NOMINA # 24 y Vacaciones Esther Morlaes Alarcon</t>
+  </si>
+  <si>
+    <t>LONGANIZA--QUESO GOUDA</t>
+  </si>
+  <si>
+    <t>NOMINA # 25</t>
   </si>
 </sst>
 </file>
@@ -10282,8 +10288,8 @@
   </sheetPr>
   <dimension ref="A1:U79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11246,35 +11252,40 @@
         <v>45100</v>
       </c>
       <c r="C23" s="25">
-        <v>0</v>
+        <v>9833</v>
       </c>
       <c r="D23" s="46"/>
       <c r="E23" s="27">
         <v>45100</v>
       </c>
-      <c r="F23" s="28"/>
+      <c r="F23" s="28">
+        <v>184445</v>
+      </c>
       <c r="G23" s="29"/>
       <c r="H23" s="30">
         <v>45100</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="31">
+        <v>204</v>
+      </c>
       <c r="J23" s="270"/>
       <c r="K23" s="271"/>
       <c r="L23" s="263"/>
       <c r="M23" s="33">
-        <v>0</v>
+        <f>15500+158659</f>
+        <v>174159</v>
       </c>
       <c r="N23" s="34">
-        <v>0</v>
+        <v>256.47000000000003</v>
       </c>
       <c r="O23" s="35"/>
       <c r="P23" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>184452.47</v>
       </c>
       <c r="Q23" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.4700000000011642</v>
       </c>
       <c r="R23" s="238">
         <v>0</v>
@@ -11287,35 +11298,48 @@
         <v>45101</v>
       </c>
       <c r="C24" s="25">
-        <v>0</v>
-      </c>
-      <c r="D24" s="42"/>
+        <v>5616</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>368</v>
+      </c>
       <c r="E24" s="27">
         <v>45101</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="28">
+        <v>114135</v>
+      </c>
       <c r="G24" s="29"/>
       <c r="H24" s="30">
         <v>45101</v>
       </c>
-      <c r="I24" s="31"/>
-      <c r="J24" s="272"/>
-      <c r="K24" s="271"/>
-      <c r="L24" s="273"/>
+      <c r="I24" s="31">
+        <v>38</v>
+      </c>
+      <c r="J24" s="272">
+        <v>45101</v>
+      </c>
+      <c r="K24" s="271" t="s">
+        <v>369</v>
+      </c>
+      <c r="L24" s="273">
+        <v>8017</v>
+      </c>
       <c r="M24" s="33">
-        <v>0</v>
+        <f>26000+73808</f>
+        <v>99808</v>
       </c>
       <c r="N24" s="34">
-        <v>0</v>
+        <v>675.88</v>
       </c>
       <c r="O24" s="35"/>
       <c r="P24" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>114154.88</v>
       </c>
       <c r="Q24" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19.880000000004657</v>
       </c>
       <c r="R24" s="238">
         <v>0</v>
@@ -11334,29 +11358,34 @@
       <c r="E25" s="27">
         <v>45102</v>
       </c>
-      <c r="F25" s="28"/>
+      <c r="F25" s="28">
+        <v>122912</v>
+      </c>
       <c r="G25" s="29"/>
       <c r="H25" s="30">
         <v>45102</v>
       </c>
-      <c r="I25" s="31"/>
+      <c r="I25" s="31">
+        <v>5</v>
+      </c>
       <c r="J25" s="274"/>
       <c r="K25" s="275"/>
       <c r="L25" s="276"/>
       <c r="M25" s="33">
-        <v>0</v>
+        <f>101000+19010+500</f>
+        <v>120510</v>
       </c>
       <c r="N25" s="34">
-        <v>0</v>
+        <v>2468.91</v>
       </c>
       <c r="O25" s="35"/>
       <c r="P25" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>122983.91</v>
       </c>
       <c r="Q25" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>71.910000000003492</v>
       </c>
       <c r="R25" s="238">
         <v>0</v>
@@ -11375,29 +11404,34 @@
       <c r="E26" s="27">
         <v>45103</v>
       </c>
-      <c r="F26" s="28"/>
+      <c r="F26" s="28">
+        <v>156919</v>
+      </c>
       <c r="G26" s="29"/>
       <c r="H26" s="30">
         <v>45103</v>
       </c>
-      <c r="I26" s="31"/>
+      <c r="I26" s="31">
+        <v>199</v>
+      </c>
       <c r="J26" s="258"/>
       <c r="K26" s="271"/>
       <c r="L26" s="263"/>
       <c r="M26" s="33">
-        <v>0</v>
+        <f>23000+133406</f>
+        <v>156406</v>
       </c>
       <c r="N26" s="34">
-        <v>0</v>
+        <v>323.42</v>
       </c>
       <c r="O26" s="35"/>
       <c r="P26" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>156928.42000000001</v>
       </c>
       <c r="Q26" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.4200000000128057</v>
       </c>
       <c r="R26" s="238">
         <v>0</v>
@@ -11410,23 +11444,28 @@
         <v>45104</v>
       </c>
       <c r="C27" s="25">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D27" s="42"/>
       <c r="E27" s="27">
         <v>45104</v>
       </c>
-      <c r="F27" s="28"/>
+      <c r="F27" s="28">
+        <v>86884</v>
+      </c>
       <c r="G27" s="29"/>
       <c r="H27" s="30">
         <v>45104</v>
       </c>
-      <c r="I27" s="31"/>
+      <c r="I27" s="31">
+        <v>144</v>
+      </c>
       <c r="J27" s="277"/>
       <c r="K27" s="275"/>
       <c r="L27" s="276"/>
       <c r="M27" s="33">
-        <v>0</v>
+        <f>54724+32000</f>
+        <v>86724</v>
       </c>
       <c r="N27" s="34">
         <v>0</v>
@@ -11434,7 +11473,7 @@
       <c r="O27" s="35"/>
       <c r="P27" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>86884</v>
       </c>
       <c r="Q27" s="236">
         <f t="shared" si="1"/>
@@ -11457,29 +11496,34 @@
       <c r="E28" s="27">
         <v>45105</v>
       </c>
-      <c r="F28" s="28"/>
+      <c r="F28" s="28">
+        <v>115082</v>
+      </c>
       <c r="G28" s="29"/>
       <c r="H28" s="30">
         <v>45105</v>
       </c>
-      <c r="I28" s="31"/>
+      <c r="I28" s="31">
+        <v>152</v>
+      </c>
       <c r="J28" s="278"/>
       <c r="K28" s="71"/>
       <c r="L28" s="276"/>
       <c r="M28" s="33">
-        <v>0</v>
+        <f>67303+47000</f>
+        <v>114303</v>
       </c>
       <c r="N28" s="34">
-        <v>0</v>
+        <v>645.80999999999995</v>
       </c>
       <c r="O28" s="35"/>
       <c r="P28" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>115100.81</v>
       </c>
       <c r="Q28" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18.809999999997672</v>
       </c>
       <c r="R28" s="238">
         <v>0</v>
@@ -11498,29 +11542,34 @@
       <c r="E29" s="27">
         <v>45106</v>
       </c>
-      <c r="F29" s="28"/>
+      <c r="F29" s="28">
+        <v>98065</v>
+      </c>
       <c r="G29" s="29"/>
       <c r="H29" s="30">
         <v>45106</v>
       </c>
-      <c r="I29" s="31"/>
+      <c r="I29" s="31">
+        <v>130</v>
+      </c>
       <c r="J29" s="277"/>
       <c r="K29" s="279"/>
       <c r="L29" s="276"/>
       <c r="M29" s="33">
-        <v>0</v>
+        <f>68310+29000</f>
+        <v>97310</v>
       </c>
       <c r="N29" s="34">
-        <v>0</v>
+        <v>643.75</v>
       </c>
       <c r="O29" s="35"/>
       <c r="P29" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>98083.75</v>
       </c>
       <c r="Q29" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>18.75</v>
       </c>
       <c r="R29" s="238">
         <v>0</v>
@@ -11534,35 +11583,42 @@
         <v>45107</v>
       </c>
       <c r="C30" s="25">
-        <v>0</v>
-      </c>
-      <c r="D30" s="72"/>
+        <v>9696</v>
+      </c>
+      <c r="D30" s="72" t="s">
+        <v>69</v>
+      </c>
       <c r="E30" s="27">
         <v>45107</v>
       </c>
-      <c r="F30" s="28"/>
+      <c r="F30" s="28">
+        <v>120962</v>
+      </c>
       <c r="G30" s="29"/>
       <c r="H30" s="30">
         <v>45107</v>
       </c>
-      <c r="I30" s="31"/>
+      <c r="I30" s="31">
+        <v>103</v>
+      </c>
       <c r="J30" s="86"/>
       <c r="K30" s="280"/>
       <c r="L30" s="281"/>
       <c r="M30" s="33">
-        <v>0</v>
+        <f>98289+12000</f>
+        <v>110289</v>
       </c>
       <c r="N30" s="34">
-        <v>0</v>
+        <v>900.22</v>
       </c>
       <c r="O30" s="35"/>
       <c r="P30" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>120988.22</v>
       </c>
       <c r="Q30" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>26.220000000001164</v>
       </c>
       <c r="R30" s="238">
         <v>0</v>
@@ -12053,19 +12109,19 @@
       <c r="L45" s="281"/>
       <c r="M45" s="351">
         <f>SUM(M5:M39)</f>
-        <v>2015658</v>
+        <v>2975167</v>
       </c>
       <c r="N45" s="336">
         <f>SUM(N5:N39)</f>
-        <v>23073.279999999999</v>
+        <v>28987.74</v>
       </c>
       <c r="P45" s="98">
         <f t="shared" si="0"/>
-        <v>2038731.28</v>
+        <v>3004154.74</v>
       </c>
       <c r="Q45" s="236">
         <f t="shared" si="1"/>
-        <v>2038731.28</v>
+        <v>3004154.74</v>
       </c>
       <c r="R45" s="99">
         <f>SUM(R5:R39)</f>
@@ -12136,7 +12192,7 @@
       </c>
       <c r="C49" s="122">
         <f>SUM(C5:C48)</f>
-        <v>42419</v>
+        <v>67580</v>
       </c>
       <c r="D49" s="123"/>
       <c r="E49" s="124" t="s">
@@ -12144,7 +12200,7 @@
       </c>
       <c r="F49" s="125">
         <f>SUM(F5:F48)</f>
-        <v>2060383</v>
+        <v>3059787</v>
       </c>
       <c r="G49" s="123"/>
       <c r="H49" s="126" t="s">
@@ -12152,7 +12208,7 @@
       </c>
       <c r="I49" s="127">
         <f>SUM(I5:I48)</f>
-        <v>2682</v>
+        <v>3657</v>
       </c>
       <c r="J49" s="290"/>
       <c r="K49" s="291" t="s">
@@ -12160,7 +12216,7 @@
       </c>
       <c r="L49" s="292">
         <f>SUM(L5:L48)</f>
-        <v>18650</v>
+        <v>26667</v>
       </c>
       <c r="M49" s="131"/>
       <c r="N49" s="131"/>
@@ -12185,12 +12241,12 @@
       <c r="J51" s="135"/>
       <c r="K51" s="340">
         <f>I49+L49</f>
-        <v>21332</v>
+        <v>30324</v>
       </c>
       <c r="L51" s="341"/>
       <c r="M51" s="342">
         <f>N45+M45</f>
-        <v>2038731.28</v>
+        <v>3004154.74</v>
       </c>
       <c r="N51" s="343"/>
       <c r="P51" s="36"/>
@@ -12203,7 +12259,7 @@
       <c r="E52" s="335"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
-        <v>1996632</v>
+        <v>2961883</v>
       </c>
       <c r="I52" s="137"/>
       <c r="J52" s="138"/>
@@ -12224,7 +12280,7 @@
       <c r="J53" s="355"/>
       <c r="K53" s="368">
         <f>F55+F56+F57</f>
-        <v>-772832.12</v>
+        <v>192418.88</v>
       </c>
       <c r="L53" s="369"/>
       <c r="P53" s="36"/>
@@ -12250,7 +12306,7 @@
       </c>
       <c r="F55" s="131">
         <f>SUM(F52:F54)</f>
-        <v>-1131940.23</v>
+        <v>-166689.22999999998</v>
       </c>
       <c r="H55" s="23"/>
       <c r="I55" s="146" t="s">
@@ -12291,7 +12347,7 @@
       <c r="J57" s="378"/>
       <c r="K57" s="379">
         <f>K53+K55</f>
-        <v>-1118465.81</v>
+        <v>-153214.81</v>
       </c>
       <c r="L57" s="379"/>
     </row>

</xml_diff>

<commit_message>
CIERRE 14 JUL 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #06  JUNIO  2023/BALANCE  HERRADURA  JUNIO    2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #06  JUNIO  2023/BALANCE  HERRADURA  JUNIO    2023.xlsx
@@ -385,7 +385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="378">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1508,6 +1508,30 @@
   </si>
   <si>
     <t>NOMINA # 25</t>
+  </si>
+  <si>
+    <t>NOMINA # 26</t>
+  </si>
+  <si>
+    <t>bancanet</t>
+  </si>
+  <si>
+    <t>comision ????</t>
+  </si>
+  <si>
+    <t>guardia junio</t>
+  </si>
+  <si>
+    <t>telmex</t>
+  </si>
+  <si>
+    <t>fumigacion</t>
+  </si>
+  <si>
+    <t>ADT SEGURITY</t>
+  </si>
+  <si>
+    <t>Comisiones banco</t>
   </si>
 </sst>
 </file>
@@ -2043,7 +2067,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="71">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -2923,12 +2947,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="382">
+  <cellXfs count="387">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3566,6 +3603,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="4" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="4" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3617,69 +3717,6 @@
     <xf numFmtId="167" fontId="14" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="4" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="4" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="10" fillId="3" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3710,12 +3747,6 @@
     <xf numFmtId="166" fontId="3" fillId="7" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="51" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="51" fillId="9" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="14" fillId="9" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3725,11 +3756,26 @@
     <xf numFmtId="166" fontId="16" fillId="9" borderId="54" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="51" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="51" fillId="9" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="51" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="51" fillId="12" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="8" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="13" fillId="13" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="13" fillId="13" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6611,23 +6657,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="339"/>
+      <c r="C1" s="341" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="342"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
+      <c r="H1" s="342"/>
+      <c r="I1" s="342"/>
+      <c r="J1" s="342"/>
+      <c r="K1" s="342"/>
+      <c r="L1" s="342"/>
+      <c r="M1" s="342"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="340"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -6637,21 +6683,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="343" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="344"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="345"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="327" t="s">
+      <c r="R3" s="348" t="s">
         <v>2</v>
       </c>
     </row>
@@ -6666,14 +6712,14 @@
       <c r="D4" s="17">
         <v>44934</v>
       </c>
-      <c r="E4" s="329" t="s">
+      <c r="E4" s="350" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="330"/>
-      <c r="H4" s="331" t="s">
+      <c r="F4" s="351"/>
+      <c r="H4" s="352" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="332"/>
+      <c r="I4" s="353"/>
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
@@ -6683,11 +6729,11 @@
       <c r="N4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="333" t="s">
+      <c r="P4" s="354" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="334"/>
-      <c r="R4" s="328"/>
+      <c r="Q4" s="355"/>
+      <c r="R4" s="349"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -8492,11 +8538,11 @@
       <c r="L49" s="76">
         <v>549</v>
       </c>
-      <c r="M49" s="351">
+      <c r="M49" s="346">
         <f>SUM(M5:M39)</f>
         <v>1666347.5</v>
       </c>
-      <c r="N49" s="336">
+      <c r="N49" s="357">
         <f>SUM(N5:N39)</f>
         <v>49399</v>
       </c>
@@ -8531,8 +8577,8 @@
       <c r="L50" s="76">
         <v>2591.1799999999998</v>
       </c>
-      <c r="M50" s="352"/>
-      <c r="N50" s="337"/>
+      <c r="M50" s="347"/>
+      <c r="N50" s="358"/>
       <c r="P50" s="36"/>
       <c r="Q50" s="9"/>
       <c r="R50" s="13">
@@ -8624,29 +8670,29 @@
       <c r="A55" s="133"/>
       <c r="B55" s="134"/>
       <c r="C55" s="1"/>
-      <c r="H55" s="338" t="s">
+      <c r="H55" s="359" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="339"/>
+      <c r="I55" s="360"/>
       <c r="J55" s="135"/>
-      <c r="K55" s="340">
+      <c r="K55" s="361">
         <f>I53+L53</f>
         <v>63475.360000000001</v>
       </c>
-      <c r="L55" s="341"/>
-      <c r="M55" s="342">
+      <c r="L55" s="362"/>
+      <c r="M55" s="363">
         <f>N49+M49</f>
         <v>1715746.5</v>
       </c>
-      <c r="N55" s="343"/>
+      <c r="N55" s="364"/>
       <c r="P55" s="36"/>
       <c r="Q55" s="9"/>
     </row>
     <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D56" s="335" t="s">
+      <c r="D56" s="356" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="335"/>
+      <c r="E56" s="356"/>
       <c r="F56" s="136">
         <f>F53-K55-C53</f>
         <v>1656897.64</v>
@@ -8657,22 +8703,22 @@
       <c r="Q56" s="9"/>
     </row>
     <row r="57" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D57" s="353" t="s">
+      <c r="D57" s="327" t="s">
         <v>15</v>
       </c>
-      <c r="E57" s="353"/>
+      <c r="E57" s="327"/>
       <c r="F57" s="131">
         <v>-1524395.48</v>
       </c>
-      <c r="I57" s="354" t="s">
+      <c r="I57" s="328" t="s">
         <v>16</v>
       </c>
-      <c r="J57" s="355"/>
-      <c r="K57" s="356">
+      <c r="J57" s="329"/>
+      <c r="K57" s="330">
         <f>F59+F60+F61</f>
         <v>393764.05999999994</v>
       </c>
-      <c r="L57" s="357"/>
+      <c r="L57" s="331"/>
       <c r="P57" s="36"/>
       <c r="Q57" s="9"/>
     </row>
@@ -8703,11 +8749,11 @@
         <v>18</v>
       </c>
       <c r="J59" s="147"/>
-      <c r="K59" s="358">
+      <c r="K59" s="332">
         <f>-C4</f>
         <v>-373948.72</v>
       </c>
-      <c r="L59" s="359"/>
+      <c r="L59" s="333"/>
     </row>
     <row r="60" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D60" s="148" t="s">
@@ -8724,22 +8770,22 @@
       <c r="C61" s="150">
         <v>44955</v>
       </c>
-      <c r="D61" s="360" t="s">
+      <c r="D61" s="334" t="s">
         <v>21</v>
       </c>
-      <c r="E61" s="361"/>
+      <c r="E61" s="335"/>
       <c r="F61" s="151">
         <v>223528.9</v>
       </c>
-      <c r="I61" s="362" t="s">
+      <c r="I61" s="336" t="s">
         <v>22</v>
       </c>
-      <c r="J61" s="363"/>
-      <c r="K61" s="364">
+      <c r="J61" s="337"/>
+      <c r="K61" s="338">
         <f>K57+K59</f>
         <v>19815.339999999967</v>
       </c>
-      <c r="L61" s="364"/>
+      <c r="L61" s="338"/>
     </row>
     <row r="62" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C62" s="152"/>
@@ -8864,18 +8910,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M49:M50"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -8885,6 +8919,18 @@
     <mergeCell ref="H55:I55"/>
     <mergeCell ref="K55:L55"/>
     <mergeCell ref="M55:N55"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="K61:L61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10288,8 +10334,8 @@
   </sheetPr>
   <dimension ref="A1:U79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10314,23 +10360,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="339"/>
+      <c r="C1" s="341" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="342"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
+      <c r="H1" s="342"/>
+      <c r="I1" s="342"/>
+      <c r="J1" s="342"/>
+      <c r="K1" s="342"/>
+      <c r="L1" s="342"/>
+      <c r="M1" s="342"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="340"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -10343,17 +10389,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="343" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="344"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="345"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
@@ -10372,14 +10418,14 @@
       <c r="D4" s="307">
         <v>45081</v>
       </c>
-      <c r="E4" s="329" t="s">
+      <c r="E4" s="350" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="330"/>
-      <c r="H4" s="331" t="s">
+      <c r="F4" s="351"/>
+      <c r="H4" s="352" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="332"/>
+      <c r="I4" s="353"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -11631,35 +11677,48 @@
         <v>45108</v>
       </c>
       <c r="C31" s="25">
-        <v>0</v>
-      </c>
-      <c r="D31" s="77"/>
+        <v>3000</v>
+      </c>
+      <c r="D31" s="77" t="s">
+        <v>67</v>
+      </c>
       <c r="E31" s="27">
         <v>45108</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="28">
+        <v>141525</v>
+      </c>
       <c r="G31" s="29"/>
       <c r="H31" s="30">
         <v>45108</v>
       </c>
-      <c r="I31" s="31"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="282"/>
-      <c r="L31" s="283"/>
+      <c r="I31" s="31">
+        <v>148</v>
+      </c>
+      <c r="J31" s="278">
+        <v>45108</v>
+      </c>
+      <c r="K31" s="275" t="s">
+        <v>370</v>
+      </c>
+      <c r="L31" s="276">
+        <v>8233</v>
+      </c>
       <c r="M31" s="33">
-        <v>0</v>
+        <f>24500+103972</f>
+        <v>128472</v>
       </c>
       <c r="N31" s="34">
-        <v>0</v>
+        <v>1722.16</v>
       </c>
       <c r="O31" s="35"/>
       <c r="P31" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>141575.16</v>
       </c>
       <c r="Q31" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>50.160000000003492</v>
       </c>
       <c r="R31" s="238">
         <v>0</v>
@@ -11678,29 +11737,34 @@
       <c r="E32" s="27">
         <v>45109</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="28">
+        <v>68123</v>
+      </c>
       <c r="G32" s="29"/>
       <c r="H32" s="30">
         <v>45109</v>
       </c>
-      <c r="I32" s="31"/>
+      <c r="I32" s="31">
+        <v>0</v>
+      </c>
       <c r="J32" s="86"/>
       <c r="K32" s="280"/>
       <c r="L32" s="281"/>
       <c r="M32" s="33">
-        <v>0</v>
+        <f>56000+11112</f>
+        <v>67112</v>
       </c>
       <c r="N32" s="34">
-        <v>0</v>
+        <v>1041.33</v>
       </c>
       <c r="O32" s="35"/>
       <c r="P32" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>68153.33</v>
       </c>
       <c r="Q32" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30.330000000001746</v>
       </c>
       <c r="R32" s="238">
         <v>0</v>
@@ -11783,9 +11847,15 @@
       <c r="G35" s="29"/>
       <c r="H35" s="30"/>
       <c r="I35" s="31"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="282"/>
-      <c r="L35" s="216"/>
+      <c r="J35" s="86">
+        <v>45083</v>
+      </c>
+      <c r="K35" s="282" t="s">
+        <v>371</v>
+      </c>
+      <c r="L35" s="216">
+        <v>365.4</v>
+      </c>
       <c r="M35" s="33">
         <v>0</v>
       </c>
@@ -11795,11 +11865,11 @@
       <c r="O35" s="35"/>
       <c r="P35" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>365.4</v>
       </c>
       <c r="Q35" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>365.4</v>
       </c>
       <c r="R35" s="238">
         <v>0</v>
@@ -11816,9 +11886,15 @@
       <c r="G36" s="29"/>
       <c r="H36" s="30"/>
       <c r="I36" s="31"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="285"/>
-      <c r="L36" s="216"/>
+      <c r="J36" s="86">
+        <v>45084</v>
+      </c>
+      <c r="K36" s="285" t="s">
+        <v>372</v>
+      </c>
+      <c r="L36" s="216">
+        <v>1225.1199999999999</v>
+      </c>
       <c r="M36" s="33">
         <v>0</v>
       </c>
@@ -11828,11 +11904,11 @@
       <c r="O36" s="35"/>
       <c r="P36" s="235">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1225.1199999999999</v>
       </c>
       <c r="Q36" s="236">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1225.1199999999999</v>
       </c>
       <c r="R36" s="238">
         <v>0</v>
@@ -11849,9 +11925,13 @@
       <c r="G37" s="29"/>
       <c r="H37" s="30"/>
       <c r="I37" s="31"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="318"/>
-      <c r="L37" s="216"/>
+      <c r="J37" s="86">
+        <v>45084</v>
+      </c>
+      <c r="K37" s="385"/>
+      <c r="L37" s="216">
+        <v>6902.3</v>
+      </c>
       <c r="M37" s="33">
         <v>0</v>
       </c>
@@ -11881,9 +11961,15 @@
       <c r="G38" s="29"/>
       <c r="H38" s="30"/>
       <c r="I38" s="31"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="282"/>
-      <c r="L38" s="216"/>
+      <c r="J38" s="86">
+        <v>45086</v>
+      </c>
+      <c r="K38" s="282" t="s">
+        <v>373</v>
+      </c>
+      <c r="L38" s="216">
+        <v>14500</v>
+      </c>
       <c r="M38" s="33">
         <v>0</v>
       </c>
@@ -11913,9 +11999,13 @@
       <c r="G39" s="29"/>
       <c r="H39" s="30"/>
       <c r="I39" s="31"/>
-      <c r="J39" s="86"/>
-      <c r="K39" s="319"/>
-      <c r="L39" s="281"/>
+      <c r="J39" s="86">
+        <v>45091</v>
+      </c>
+      <c r="K39" s="386"/>
+      <c r="L39" s="281">
+        <v>522</v>
+      </c>
       <c r="M39" s="33">
         <v>0</v>
       </c>
@@ -11945,9 +12035,15 @@
       <c r="G40" s="29"/>
       <c r="H40" s="30"/>
       <c r="I40" s="31"/>
-      <c r="J40" s="86"/>
-      <c r="K40" s="231"/>
-      <c r="L40" s="281"/>
+      <c r="J40" s="86">
+        <v>45093</v>
+      </c>
+      <c r="K40" s="231" t="s">
+        <v>374</v>
+      </c>
+      <c r="L40" s="281">
+        <v>664</v>
+      </c>
       <c r="M40" s="33">
         <v>0</v>
       </c>
@@ -11977,9 +12073,15 @@
       <c r="G41" s="29"/>
       <c r="H41" s="30"/>
       <c r="I41" s="31"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="305"/>
-      <c r="L41" s="281"/>
+      <c r="J41" s="86">
+        <v>45097</v>
+      </c>
+      <c r="K41" s="305" t="s">
+        <v>375</v>
+      </c>
+      <c r="L41" s="281">
+        <v>1392</v>
+      </c>
       <c r="M41" s="33">
         <v>0</v>
       </c>
@@ -12009,9 +12111,15 @@
       <c r="G42" s="29"/>
       <c r="H42" s="30"/>
       <c r="I42" s="31"/>
-      <c r="J42" s="86"/>
-      <c r="K42" s="231"/>
-      <c r="L42" s="281"/>
+      <c r="J42" s="86">
+        <v>45105</v>
+      </c>
+      <c r="K42" s="231" t="s">
+        <v>376</v>
+      </c>
+      <c r="L42" s="281">
+        <v>1031.47</v>
+      </c>
       <c r="M42" s="33">
         <v>0</v>
       </c>
@@ -12041,9 +12149,15 @@
       <c r="G43" s="29"/>
       <c r="H43" s="30"/>
       <c r="I43" s="91"/>
-      <c r="J43" s="86"/>
-      <c r="K43" s="89"/>
-      <c r="L43" s="281"/>
+      <c r="J43" s="86">
+        <v>45107</v>
+      </c>
+      <c r="K43" s="89" t="s">
+        <v>377</v>
+      </c>
+      <c r="L43" s="281">
+        <v>786.07</v>
+      </c>
       <c r="M43" s="33">
         <v>0</v>
       </c>
@@ -12085,7 +12199,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q44" s="236">
+      <c r="Q44" s="382">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -12107,23 +12221,23 @@
       <c r="J45" s="86"/>
       <c r="K45" s="89"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="351">
+      <c r="M45" s="346">
         <f>SUM(M5:M39)</f>
-        <v>2975167</v>
-      </c>
-      <c r="N45" s="336">
+        <v>3170751</v>
+      </c>
+      <c r="N45" s="357">
         <f>SUM(N5:N39)</f>
-        <v>28987.74</v>
+        <v>31751.230000000003</v>
       </c>
       <c r="P45" s="98">
         <f t="shared" si="0"/>
-        <v>3004154.74</v>
-      </c>
-      <c r="Q45" s="236">
-        <f t="shared" si="1"/>
-        <v>3004154.74</v>
-      </c>
-      <c r="R45" s="99">
+        <v>3202502.23</v>
+      </c>
+      <c r="Q45" s="383">
+        <f>SUM(Q21:Q44)</f>
+        <v>1843.4700000000262</v>
+      </c>
+      <c r="R45" s="384">
         <f>SUM(R5:R39)</f>
         <v>41424</v>
       </c>
@@ -12141,8 +12255,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="337"/>
+      <c r="M46" s="347"/>
+      <c r="N46" s="358"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -12192,7 +12306,7 @@
       </c>
       <c r="C49" s="122">
         <f>SUM(C5:C48)</f>
-        <v>67580</v>
+        <v>70580</v>
       </c>
       <c r="D49" s="123"/>
       <c r="E49" s="124" t="s">
@@ -12200,7 +12314,7 @@
       </c>
       <c r="F49" s="125">
         <f>SUM(F5:F48)</f>
-        <v>3059787</v>
+        <v>3269435</v>
       </c>
       <c r="G49" s="123"/>
       <c r="H49" s="126" t="s">
@@ -12208,7 +12322,7 @@
       </c>
       <c r="I49" s="127">
         <f>SUM(I5:I48)</f>
-        <v>3657</v>
+        <v>3805</v>
       </c>
       <c r="J49" s="290"/>
       <c r="K49" s="291" t="s">
@@ -12216,7 +12330,7 @@
       </c>
       <c r="L49" s="292">
         <f>SUM(L5:L48)</f>
-        <v>26667</v>
+        <v>62288.360000000008</v>
       </c>
       <c r="M49" s="131"/>
       <c r="N49" s="131"/>
@@ -12234,32 +12348,32 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="338" t="s">
+      <c r="H51" s="359" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="339"/>
+      <c r="I51" s="360"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="340">
+      <c r="K51" s="361">
         <f>I49+L49</f>
-        <v>30324</v>
-      </c>
-      <c r="L51" s="341"/>
-      <c r="M51" s="342">
+        <v>66093.360000000015</v>
+      </c>
+      <c r="L51" s="362"/>
+      <c r="M51" s="363">
         <f>N45+M45</f>
-        <v>3004154.74</v>
-      </c>
-      <c r="N51" s="343"/>
+        <v>3202502.23</v>
+      </c>
+      <c r="N51" s="364"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="335" t="s">
+      <c r="D52" s="356" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="335"/>
+      <c r="E52" s="356"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
-        <v>2961883</v>
+        <v>3132761.64</v>
       </c>
       <c r="I52" s="137"/>
       <c r="J52" s="138"/>
@@ -12267,20 +12381,20 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="353" t="s">
+      <c r="D53" s="327" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="353"/>
+      <c r="E53" s="327"/>
       <c r="F53" s="131">
         <v>-3128572.23</v>
       </c>
-      <c r="I53" s="354" t="s">
+      <c r="I53" s="328" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="355"/>
+      <c r="J53" s="329"/>
       <c r="K53" s="368">
         <f>F55+F56+F57</f>
-        <v>192418.88</v>
+        <v>417897.52000000014</v>
       </c>
       <c r="L53" s="369"/>
       <c r="P53" s="36"/>
@@ -12306,7 +12420,7 @@
       </c>
       <c r="F55" s="131">
         <f>SUM(F52:F54)</f>
-        <v>-166689.22999999998</v>
+        <v>4189.410000000149</v>
       </c>
       <c r="H55" s="23"/>
       <c r="I55" s="146" t="s">
@@ -12327,29 +12441,29 @@
         <v>20</v>
       </c>
       <c r="F56" s="149">
-        <v>0</v>
+        <v>54600</v>
       </c>
     </row>
     <row r="57" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C57" s="150">
         <v>45109</v>
       </c>
-      <c r="D57" s="360" t="s">
+      <c r="D57" s="334" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="361"/>
+      <c r="E57" s="335"/>
       <c r="F57" s="316">
         <v>359108.11</v>
       </c>
-      <c r="I57" s="377" t="s">
+      <c r="I57" s="375" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="378"/>
-      <c r="K57" s="379">
+      <c r="J57" s="376"/>
+      <c r="K57" s="377">
         <f>K53+K55</f>
-        <v>-153214.81</v>
-      </c>
-      <c r="L57" s="379"/>
+        <v>72263.830000000133</v>
+      </c>
+      <c r="L57" s="377"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -12474,6 +12588,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -12483,22 +12609,11 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -15254,23 +15369,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="339"/>
+      <c r="C1" s="341" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="342"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
+      <c r="H1" s="342"/>
+      <c r="I1" s="342"/>
+      <c r="J1" s="342"/>
+      <c r="K1" s="342"/>
+      <c r="L1" s="342"/>
+      <c r="M1" s="342"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="340"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -15280,21 +15395,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="343" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="344"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="345"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="327" t="s">
+      <c r="R3" s="348" t="s">
         <v>2</v>
       </c>
     </row>
@@ -15309,14 +15424,14 @@
       <c r="D4" s="17">
         <v>44955</v>
       </c>
-      <c r="E4" s="329" t="s">
+      <c r="E4" s="350" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="330"/>
-      <c r="H4" s="331" t="s">
+      <c r="F4" s="351"/>
+      <c r="H4" s="352" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="332"/>
+      <c r="I4" s="353"/>
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
@@ -17131,11 +17246,11 @@
       <c r="J45" s="74"/>
       <c r="K45" s="97"/>
       <c r="L45" s="76"/>
-      <c r="M45" s="351">
+      <c r="M45" s="346">
         <f>SUM(M5:M39)</f>
         <v>2238523</v>
       </c>
-      <c r="N45" s="336">
+      <c r="N45" s="357">
         <f>SUM(N5:N39)</f>
         <v>97258</v>
       </c>
@@ -17165,8 +17280,8 @@
       <c r="J46" s="74"/>
       <c r="K46" s="102"/>
       <c r="L46" s="76"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="337"/>
+      <c r="M46" s="347"/>
+      <c r="N46" s="358"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -17258,29 +17373,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="338" t="s">
+      <c r="H51" s="359" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="339"/>
+      <c r="I51" s="360"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="340">
+      <c r="K51" s="361">
         <f>I49+L49</f>
         <v>90767.040000000008</v>
       </c>
-      <c r="L51" s="341"/>
-      <c r="M51" s="342">
+      <c r="L51" s="362"/>
+      <c r="M51" s="363">
         <f>N45+M45</f>
         <v>2335781</v>
       </c>
-      <c r="N51" s="343"/>
+      <c r="N51" s="364"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D52" s="335" t="s">
+      <c r="D52" s="356" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="335"/>
+      <c r="E52" s="356"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2261973.96</v>
@@ -17291,22 +17406,22 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D53" s="353" t="s">
+      <c r="D53" s="327" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="353"/>
+      <c r="E53" s="327"/>
       <c r="F53" s="131">
         <v>-2224189.7400000002</v>
       </c>
-      <c r="I53" s="354" t="s">
+      <c r="I53" s="328" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="355"/>
-      <c r="K53" s="356">
+      <c r="J53" s="329"/>
+      <c r="K53" s="330">
         <f>F55+F56+F57</f>
         <v>296963.76999999973</v>
       </c>
-      <c r="L53" s="357"/>
+      <c r="L53" s="331"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="9"/>
     </row>
@@ -17337,11 +17452,11 @@
         <v>18</v>
       </c>
       <c r="J55" s="147"/>
-      <c r="K55" s="358">
+      <c r="K55" s="332">
         <f>-C4</f>
         <v>-223528.9</v>
       </c>
-      <c r="L55" s="359"/>
+      <c r="L55" s="333"/>
     </row>
     <row r="56" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="148" t="s">
@@ -17358,22 +17473,22 @@
       <c r="C57" s="150">
         <v>44985</v>
       </c>
-      <c r="D57" s="360" t="s">
+      <c r="D57" s="334" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="361"/>
+      <c r="E57" s="335"/>
       <c r="F57" s="151">
         <v>230554.55</v>
       </c>
-      <c r="I57" s="362" t="s">
+      <c r="I57" s="336" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="363"/>
-      <c r="K57" s="364">
+      <c r="J57" s="337"/>
+      <c r="K57" s="338">
         <f>K53+K55</f>
         <v>73434.869999999733</v>
       </c>
-      <c r="L57" s="364"/>
+      <c r="L57" s="338"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -17498,18 +17613,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -17519,6 +17622,18 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -18977,23 +19092,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="339"/>
+      <c r="C1" s="341" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="342"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
+      <c r="H1" s="342"/>
+      <c r="I1" s="342"/>
+      <c r="J1" s="342"/>
+      <c r="K1" s="342"/>
+      <c r="L1" s="342"/>
+      <c r="M1" s="342"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="340"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -19003,21 +19118,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="343" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="344"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="345"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="327" t="s">
+      <c r="R3" s="348" t="s">
         <v>2</v>
       </c>
     </row>
@@ -19032,14 +19147,14 @@
       <c r="D4" s="17">
         <v>44985</v>
       </c>
-      <c r="E4" s="329" t="s">
+      <c r="E4" s="350" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="330"/>
-      <c r="H4" s="331" t="s">
+      <c r="F4" s="351"/>
+      <c r="H4" s="352" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="332"/>
+      <c r="I4" s="353"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -20846,11 +20961,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="231"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="351">
+      <c r="M45" s="346">
         <f>SUM(M5:M39)</f>
         <v>2689952</v>
       </c>
-      <c r="N45" s="336">
+      <c r="N45" s="357">
         <f>SUM(N5:N39)</f>
         <v>61422</v>
       </c>
@@ -20880,8 +20995,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="337"/>
+      <c r="M46" s="347"/>
+      <c r="N46" s="358"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -20973,29 +21088,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="338" t="s">
+      <c r="H51" s="359" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="339"/>
+      <c r="I51" s="360"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="340">
+      <c r="K51" s="361">
         <f>I49+L49</f>
         <v>425400.67</v>
       </c>
-      <c r="L51" s="341"/>
-      <c r="M51" s="342">
+      <c r="L51" s="362"/>
+      <c r="M51" s="363">
         <f>N45+M45</f>
         <v>2751374</v>
       </c>
-      <c r="N51" s="343"/>
+      <c r="N51" s="364"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="335" t="s">
+      <c r="D52" s="356" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="335"/>
+      <c r="E52" s="356"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2464124.33</v>
@@ -21006,17 +21121,17 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="353" t="s">
+      <c r="D53" s="327" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="353"/>
+      <c r="E53" s="327"/>
       <c r="F53" s="131">
         <v>-2869426.04</v>
       </c>
-      <c r="I53" s="354" t="s">
+      <c r="I53" s="328" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="355"/>
+      <c r="J53" s="329"/>
       <c r="K53" s="368">
         <f>F55+F56+F57</f>
         <v>-32021.369999999937</v>
@@ -21073,10 +21188,10 @@
       <c r="C57" s="150">
         <v>45015</v>
       </c>
-      <c r="D57" s="360" t="s">
+      <c r="D57" s="334" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="361"/>
+      <c r="E57" s="335"/>
       <c r="F57" s="151">
         <v>341192.34</v>
       </c>
@@ -21213,6 +21328,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -21222,18 +21349,6 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22635,23 +22750,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="339"/>
+      <c r="C1" s="341" t="s">
         <v>171</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="342"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
+      <c r="H1" s="342"/>
+      <c r="I1" s="342"/>
+      <c r="J1" s="342"/>
+      <c r="K1" s="342"/>
+      <c r="L1" s="342"/>
+      <c r="M1" s="342"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="340"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -22664,21 +22779,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="343" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="344"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="345"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
-      <c r="R3" s="375" t="s">
+      <c r="R3" s="378" t="s">
         <v>2</v>
       </c>
     </row>
@@ -22693,14 +22808,14 @@
       <c r="D4" s="17">
         <v>45015</v>
       </c>
-      <c r="E4" s="329" t="s">
+      <c r="E4" s="350" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="330"/>
-      <c r="H4" s="331" t="s">
+      <c r="F4" s="351"/>
+      <c r="H4" s="352" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="332"/>
+      <c r="I4" s="353"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -22714,7 +22829,7 @@
         <v>8</v>
       </c>
       <c r="Q4" s="367"/>
-      <c r="R4" s="376"/>
+      <c r="R4" s="379"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -24601,11 +24716,11 @@
       <c r="L45" s="312">
         <v>2123.98</v>
       </c>
-      <c r="M45" s="351">
+      <c r="M45" s="346">
         <f>SUM(M5:M39)</f>
         <v>2488709</v>
       </c>
-      <c r="N45" s="336">
+      <c r="N45" s="357">
         <f>SUM(N5:N39)</f>
         <v>78710</v>
       </c>
@@ -24641,8 +24756,8 @@
       <c r="L46" s="281">
         <v>34015</v>
       </c>
-      <c r="M46" s="352"/>
-      <c r="N46" s="337"/>
+      <c r="M46" s="347"/>
+      <c r="N46" s="358"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -24734,29 +24849,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="338" t="s">
+      <c r="H51" s="359" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="339"/>
+      <c r="I51" s="360"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="340">
+      <c r="K51" s="361">
         <f>I49+L49</f>
         <v>124244.06999999999</v>
       </c>
-      <c r="L51" s="341"/>
-      <c r="M51" s="342">
+      <c r="L51" s="362"/>
+      <c r="M51" s="363">
         <f>N45+M45</f>
         <v>2567419</v>
       </c>
-      <c r="N51" s="343"/>
+      <c r="N51" s="364"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="335" t="s">
+      <c r="D52" s="356" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="335"/>
+      <c r="E52" s="356"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2480239.9300000002</v>
@@ -24767,17 +24882,17 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="353" t="s">
+      <c r="D53" s="327" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="353"/>
+      <c r="E53" s="327"/>
       <c r="F53" s="131">
         <v>-2463938.5299999998</v>
       </c>
-      <c r="I53" s="354" t="s">
+      <c r="I53" s="328" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="355"/>
+      <c r="J53" s="329"/>
       <c r="K53" s="368">
         <f>F55+F56+F57</f>
         <v>439109.10000000038</v>
@@ -24834,22 +24949,22 @@
       <c r="C57" s="150">
         <v>45050</v>
       </c>
-      <c r="D57" s="360" t="s">
+      <c r="D57" s="334" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="361"/>
+      <c r="E57" s="335"/>
       <c r="F57" s="151">
         <v>394548.7</v>
       </c>
-      <c r="I57" s="377" t="s">
+      <c r="I57" s="375" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="378"/>
-      <c r="K57" s="379">
+      <c r="J57" s="376"/>
+      <c r="K57" s="377">
         <f>K53+K55</f>
         <v>97916.760000000359</v>
       </c>
-      <c r="L57" s="379"/>
+      <c r="L57" s="377"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -24974,18 +25089,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -24995,6 +25098,18 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -26386,23 +26501,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="344"/>
-      <c r="C1" s="346" t="s">
+      <c r="B1" s="339"/>
+      <c r="C1" s="341" t="s">
         <v>231</v>
       </c>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
+      <c r="D1" s="342"/>
+      <c r="E1" s="342"/>
+      <c r="F1" s="342"/>
+      <c r="G1" s="342"/>
+      <c r="H1" s="342"/>
+      <c r="I1" s="342"/>
+      <c r="J1" s="342"/>
+      <c r="K1" s="342"/>
+      <c r="L1" s="342"/>
+      <c r="M1" s="342"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="345"/>
+      <c r="B2" s="340"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
@@ -26415,17 +26530,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="348" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="349"/>
+      <c r="B3" s="343" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="344"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="345" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="350"/>
+      <c r="I3" s="345"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
@@ -26444,14 +26559,14 @@
       <c r="D4" s="307">
         <v>45050</v>
       </c>
-      <c r="E4" s="329" t="s">
+      <c r="E4" s="350" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="330"/>
-      <c r="H4" s="331" t="s">
+      <c r="F4" s="351"/>
+      <c r="H4" s="352" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="332"/>
+      <c r="I4" s="353"/>
       <c r="J4" s="255"/>
       <c r="K4" s="256"/>
       <c r="L4" s="16"/>
@@ -28338,11 +28453,11 @@
       <c r="J45" s="86"/>
       <c r="K45" s="89"/>
       <c r="L45" s="281"/>
-      <c r="M45" s="351">
+      <c r="M45" s="346">
         <f>SUM(M5:M39)</f>
         <v>3007589</v>
       </c>
-      <c r="N45" s="336">
+      <c r="N45" s="357">
         <f>SUM(N5:N39)</f>
         <v>29752</v>
       </c>
@@ -28372,8 +28487,8 @@
       <c r="J46" s="86"/>
       <c r="K46" s="102"/>
       <c r="L46" s="281"/>
-      <c r="M46" s="352"/>
-      <c r="N46" s="337"/>
+      <c r="M46" s="347"/>
+      <c r="N46" s="358"/>
       <c r="P46" s="36"/>
       <c r="Q46" s="9"/>
       <c r="R46" s="13">
@@ -28465,29 +28580,29 @@
       <c r="A51" s="133"/>
       <c r="B51" s="134"/>
       <c r="C51" s="1"/>
-      <c r="H51" s="338" t="s">
+      <c r="H51" s="359" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="339"/>
+      <c r="I51" s="360"/>
       <c r="J51" s="135"/>
-      <c r="K51" s="340">
+      <c r="K51" s="361">
         <f>I49+L49</f>
         <v>84500.43</v>
       </c>
-      <c r="L51" s="341"/>
-      <c r="M51" s="342">
+      <c r="L51" s="362"/>
+      <c r="M51" s="363">
         <f>N45+M45</f>
         <v>3037341</v>
       </c>
-      <c r="N51" s="343"/>
+      <c r="N51" s="364"/>
       <c r="P51" s="36"/>
       <c r="Q51" s="9"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D52" s="335" t="s">
+      <c r="D52" s="356" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="335"/>
+      <c r="E52" s="356"/>
       <c r="F52" s="136">
         <f>F49-K51-C49</f>
         <v>2988109.57</v>
@@ -28498,17 +28613,17 @@
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D53" s="353" t="s">
+      <c r="D53" s="327" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="353"/>
+      <c r="E53" s="327"/>
       <c r="F53" s="131">
         <v>-2955802.29</v>
       </c>
-      <c r="I53" s="354" t="s">
+      <c r="I53" s="328" t="s">
         <v>16</v>
       </c>
-      <c r="J53" s="355"/>
+      <c r="J53" s="329"/>
       <c r="K53" s="368">
         <f>F55+F56+F57</f>
         <v>419364.9699999998</v>
@@ -28565,22 +28680,22 @@
       <c r="C57" s="150">
         <v>45081</v>
       </c>
-      <c r="D57" s="360" t="s">
+      <c r="D57" s="334" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="361"/>
+      <c r="E57" s="335"/>
       <c r="F57" s="316">
         <v>345633.69</v>
       </c>
-      <c r="I57" s="377" t="s">
+      <c r="I57" s="375" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="378"/>
-      <c r="K57" s="379">
+      <c r="J57" s="376"/>
+      <c r="K57" s="377">
         <f>K53+K55</f>
         <v>24816.269999999786</v>
       </c>
-      <c r="L57" s="379"/>
+      <c r="L57" s="377"/>
     </row>
     <row r="58" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C58" s="152"/>
@@ -28705,6 +28820,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="M45:M46"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -28714,18 +28841,6 @@
     <mergeCell ref="H51:I51"/>
     <mergeCell ref="K51:L51"/>
     <mergeCell ref="M51:N51"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="90" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>